<commit_message>
template 4, TBI : midspan join, better cut when cum_span>3600 just at the last tower
</commit_message>
<xml_diff>
--- a/templates/output/template4.xlsx
+++ b/templates/output/template4.xlsx
@@ -1052,12 +1052,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1067,6 +1061,162 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1136,157 +1286,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5098,7 +5098,7 @@
   <dimension ref="A1:AI55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43:G43"/>
+      <selection activeCell="E36" sqref="E36:AD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5114,67 +5114,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108"/>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="108"/>
-      <c r="AB1" s="108"/>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="158"/>
+      <c r="O1" s="158"/>
+      <c r="P1" s="158"/>
+      <c r="Q1" s="158"/>
+      <c r="R1" s="158"/>
+      <c r="S1" s="158"/>
+      <c r="T1" s="158"/>
+      <c r="U1" s="158"/>
+      <c r="V1" s="158"/>
+      <c r="W1" s="158"/>
+      <c r="X1" s="158"/>
+      <c r="Y1" s="158"/>
+      <c r="Z1" s="158"/>
+      <c r="AA1" s="158"/>
+      <c r="AB1" s="158"/>
+      <c r="AC1" s="158"/>
+      <c r="AD1" s="158"/>
       <c r="AE1" s="86"/>
     </row>
     <row r="2" spans="1:31" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="135"/>
-      <c r="B2" s="136"/>
+      <c r="A2" s="151"/>
+      <c r="B2" s="152"/>
       <c r="C2" s="94"/>
       <c r="D2" s="95"/>
-      <c r="E2" s="114" t="s">
+      <c r="E2" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="126" t="s">
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
+      <c r="S2" s="165"/>
+      <c r="T2" s="166"/>
+      <c r="U2" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="126"/>
+      <c r="V2" s="176"/>
       <c r="W2" s="87" t="s">
         <v>11</v>
       </c>
@@ -5188,29 +5188,29 @@
       <c r="AE2" s="86"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="137"/>
-      <c r="B3" s="138"/>
+      <c r="A3" s="153"/>
+      <c r="B3" s="154"/>
       <c r="C3" s="93"/>
       <c r="D3" s="96"/>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="167" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="118"/>
-      <c r="J3" s="118"/>
-      <c r="K3" s="118"/>
-      <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="118"/>
-      <c r="P3" s="118"/>
-      <c r="Q3" s="118"/>
-      <c r="R3" s="118"/>
-      <c r="S3" s="118"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="101"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="168"/>
+      <c r="M3" s="168"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="168"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="168"/>
+      <c r="R3" s="168"/>
+      <c r="S3" s="168"/>
+      <c r="T3" s="169"/>
+      <c r="U3" s="99"/>
       <c r="W3" s="88"/>
       <c r="X3" s="88"/>
       <c r="Y3" s="88"/>
@@ -5222,32 +5222,32 @@
       <c r="AE3" s="86"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="137"/>
-      <c r="B4" s="138"/>
+      <c r="A4" s="153"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="93"/>
       <c r="D4" s="96"/>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="170" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="121"/>
-      <c r="O4" s="121"/>
-      <c r="P4" s="121"/>
-      <c r="Q4" s="121"/>
-      <c r="R4" s="121"/>
-      <c r="S4" s="121"/>
-      <c r="T4" s="122"/>
-      <c r="U4" s="126" t="s">
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="171"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="171"/>
+      <c r="S4" s="171"/>
+      <c r="T4" s="172"/>
+      <c r="U4" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="126"/>
+      <c r="V4" s="176"/>
       <c r="W4" s="87" t="s">
         <v>14</v>
       </c>
@@ -5261,30 +5261,30 @@
       <c r="AE4" s="86"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="137"/>
-      <c r="B5" s="138"/>
+      <c r="A5" s="153"/>
+      <c r="B5" s="154"/>
       <c r="C5" s="93"/>
       <c r="D5" s="96"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="106"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="126" t="s">
+      <c r="E5" s="100"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="105"/>
+      <c r="U5" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="V5" s="126"/>
+      <c r="V5" s="176"/>
       <c r="W5" s="83" t="s">
         <v>16</v>
       </c>
@@ -5300,28 +5300,28 @@
       <c r="AE5" s="86"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="137"/>
-      <c r="B6" s="138"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="154"/>
       <c r="C6" s="93"/>
       <c r="D6" s="96"/>
-      <c r="E6" s="117" t="s">
+      <c r="E6" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="119"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
+      <c r="R6" s="168"/>
+      <c r="S6" s="168"/>
+      <c r="T6" s="169"/>
       <c r="U6" s="85"/>
       <c r="V6" s="85"/>
       <c r="W6" s="85"/>
@@ -5339,68 +5339,68 @@
       <c r="B7" s="93"/>
       <c r="C7" s="93"/>
       <c r="D7" s="98"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="121"/>
-      <c r="L7" s="121"/>
-      <c r="M7" s="121"/>
-      <c r="N7" s="121"/>
-      <c r="O7" s="121"/>
-      <c r="P7" s="121"/>
-      <c r="Q7" s="121"/>
-      <c r="R7" s="121"/>
-      <c r="S7" s="121"/>
-      <c r="T7" s="122"/>
-      <c r="U7" s="109" t="s">
+      <c r="E7" s="170"/>
+      <c r="F7" s="171"/>
+      <c r="G7" s="171"/>
+      <c r="H7" s="171"/>
+      <c r="I7" s="171"/>
+      <c r="J7" s="171"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="171"/>
+      <c r="M7" s="171"/>
+      <c r="N7" s="171"/>
+      <c r="O7" s="171"/>
+      <c r="P7" s="171"/>
+      <c r="Q7" s="171"/>
+      <c r="R7" s="171"/>
+      <c r="S7" s="171"/>
+      <c r="T7" s="172"/>
+      <c r="U7" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="V7" s="110"/>
+      <c r="V7" s="160"/>
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
-      <c r="Z7" s="111" t="s">
+      <c r="Z7" s="161" t="s">
         <v>21</v>
       </c>
-      <c r="AA7" s="112"/>
+      <c r="AA7" s="162"/>
       <c r="AB7" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="128"/>
+      <c r="AC7" s="177"/>
+      <c r="AD7" s="178"/>
       <c r="AE7" s="86"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="139"/>
-      <c r="B8" s="140"/>
-      <c r="C8" s="140"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="124"/>
-      <c r="R8" s="124"/>
-      <c r="S8" s="124"/>
-      <c r="T8" s="125"/>
-      <c r="U8" s="113"/>
-      <c r="V8" s="110"/>
+      <c r="A8" s="155"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="173"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="174"/>
+      <c r="J8" s="174"/>
+      <c r="K8" s="174"/>
+      <c r="L8" s="174"/>
+      <c r="M8" s="174"/>
+      <c r="N8" s="174"/>
+      <c r="O8" s="174"/>
+      <c r="P8" s="174"/>
+      <c r="Q8" s="174"/>
+      <c r="R8" s="174"/>
+      <c r="S8" s="174"/>
+      <c r="T8" s="175"/>
+      <c r="U8" s="163"/>
+      <c r="V8" s="160"/>
       <c r="W8"/>
       <c r="X8"/>
       <c r="Y8"/>
-      <c r="Z8" s="129"/>
-      <c r="AA8" s="130"/>
+      <c r="Z8" s="179"/>
+      <c r="AA8" s="180"/>
       <c r="AB8" s="90"/>
       <c r="AC8" s="91"/>
       <c r="AD8" s="92"/>
@@ -5411,8 +5411,8 @@
       <c r="B9" s="2"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="147"/>
+      <c r="F9" s="147"/>
       <c r="G9" s="43"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -5540,9 +5540,9 @@
     </row>
     <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="55"/>
-      <c r="B13" s="132"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="132"/>
+      <c r="B13" s="148"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="148"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -5552,18 +5552,18 @@
       <c r="K13" s="27"/>
       <c r="L13" s="23"/>
       <c r="M13" s="25"/>
-      <c r="N13" s="133"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="134"/>
-      <c r="R13" s="133"/>
-      <c r="S13" s="134"/>
-      <c r="T13" s="133"/>
-      <c r="U13" s="134"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="134"/>
-      <c r="X13" s="133"/>
-      <c r="Y13" s="134"/>
+      <c r="N13" s="149"/>
+      <c r="O13" s="150"/>
+      <c r="P13" s="149"/>
+      <c r="Q13" s="150"/>
+      <c r="R13" s="149"/>
+      <c r="S13" s="150"/>
+      <c r="T13" s="149"/>
+      <c r="U13" s="150"/>
+      <c r="V13" s="149"/>
+      <c r="W13" s="150"/>
+      <c r="X13" s="149"/>
+      <c r="Y13" s="150"/>
       <c r="Z13" s="23"/>
       <c r="AA13" s="25"/>
       <c r="AB13" s="23"/>
@@ -5644,34 +5644,34 @@
       </c>
       <c r="C16" s="51"/>
       <c r="D16" s="51"/>
-      <c r="E16" s="142">
+      <c r="E16" s="117">
         <v>1</v>
       </c>
-      <c r="F16" s="148"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="148"/>
-      <c r="M16" s="142"/>
-      <c r="N16" s="148"/>
-      <c r="O16" s="142"/>
-      <c r="P16" s="148"/>
-      <c r="Q16" s="142"/>
-      <c r="R16" s="148"/>
-      <c r="S16" s="142"/>
-      <c r="T16" s="148"/>
-      <c r="U16" s="142"/>
-      <c r="V16" s="148"/>
-      <c r="W16" s="142"/>
-      <c r="X16" s="148"/>
-      <c r="Y16" s="142"/>
-      <c r="Z16" s="148"/>
-      <c r="AA16" s="142"/>
-      <c r="AB16" s="148"/>
-      <c r="AC16" s="142"/>
-      <c r="AD16" s="143"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="117"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="117"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="117"/>
+      <c r="P16" s="118"/>
+      <c r="Q16" s="117"/>
+      <c r="R16" s="118"/>
+      <c r="S16" s="117"/>
+      <c r="T16" s="118"/>
+      <c r="U16" s="117"/>
+      <c r="V16" s="118"/>
+      <c r="W16" s="117"/>
+      <c r="X16" s="118"/>
+      <c r="Y16" s="117"/>
+      <c r="Z16" s="118"/>
+      <c r="AA16" s="117"/>
+      <c r="AB16" s="118"/>
+      <c r="AC16" s="117"/>
+      <c r="AD16" s="146"/>
       <c r="AE16" s="63"/>
     </row>
     <row r="17" spans="1:34" ht="15.6" x14ac:dyDescent="0.25">
@@ -5685,30 +5685,30 @@
         <v>24</v>
       </c>
       <c r="F17" s="145"/>
-      <c r="G17" s="146"/>
-      <c r="H17" s="147"/>
-      <c r="I17" s="146"/>
-      <c r="J17" s="147"/>
-      <c r="K17" s="146"/>
-      <c r="L17" s="147"/>
-      <c r="M17" s="146"/>
-      <c r="N17" s="147"/>
-      <c r="O17" s="146"/>
-      <c r="P17" s="147"/>
-      <c r="Q17" s="146"/>
-      <c r="R17" s="147"/>
-      <c r="S17" s="146"/>
-      <c r="T17" s="147"/>
-      <c r="U17" s="146"/>
-      <c r="V17" s="147"/>
-      <c r="W17" s="146"/>
-      <c r="X17" s="147"/>
-      <c r="Y17" s="146"/>
-      <c r="Z17" s="147"/>
-      <c r="AA17" s="146"/>
-      <c r="AB17" s="147"/>
-      <c r="AC17" s="146"/>
-      <c r="AD17" s="147"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="110"/>
+      <c r="O17" s="109"/>
+      <c r="P17" s="110"/>
+      <c r="Q17" s="109"/>
+      <c r="R17" s="110"/>
+      <c r="S17" s="109"/>
+      <c r="T17" s="110"/>
+      <c r="U17" s="109"/>
+      <c r="V17" s="110"/>
+      <c r="W17" s="109"/>
+      <c r="X17" s="110"/>
+      <c r="Y17" s="109"/>
+      <c r="Z17" s="110"/>
+      <c r="AA17" s="109"/>
+      <c r="AB17" s="110"/>
+      <c r="AC17" s="109"/>
+      <c r="AD17" s="110"/>
       <c r="AE17" s="63"/>
       <c r="AG17" s="79"/>
     </row>
@@ -5719,34 +5719,34 @@
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
-      <c r="E18" s="99" t="s">
+      <c r="E18" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="100"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="99"/>
-      <c r="N18" s="100"/>
-      <c r="O18" s="99"/>
-      <c r="P18" s="100"/>
-      <c r="Q18" s="99"/>
-      <c r="R18" s="100"/>
-      <c r="S18" s="99"/>
-      <c r="T18" s="100"/>
-      <c r="U18" s="99"/>
-      <c r="V18" s="100"/>
-      <c r="W18" s="99"/>
-      <c r="X18" s="100"/>
-      <c r="Y18" s="99"/>
-      <c r="Z18" s="100"/>
-      <c r="AA18" s="99"/>
-      <c r="AB18" s="100"/>
-      <c r="AC18" s="99"/>
-      <c r="AD18" s="100"/>
+      <c r="F18" s="181"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="181"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="181"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="181"/>
+      <c r="M18" s="106"/>
+      <c r="N18" s="181"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="181"/>
+      <c r="Q18" s="106"/>
+      <c r="R18" s="181"/>
+      <c r="S18" s="106"/>
+      <c r="T18" s="181"/>
+      <c r="U18" s="106"/>
+      <c r="V18" s="181"/>
+      <c r="W18" s="106"/>
+      <c r="X18" s="181"/>
+      <c r="Y18" s="106"/>
+      <c r="Z18" s="181"/>
+      <c r="AA18" s="106"/>
+      <c r="AB18" s="181"/>
+      <c r="AC18" s="106"/>
+      <c r="AD18" s="181"/>
       <c r="AE18" s="63"/>
     </row>
     <row r="19" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5757,34 +5757,34 @@
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="54"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="152"/>
-      <c r="H19" s="151"/>
-      <c r="I19" s="152"/>
-      <c r="J19" s="151"/>
-      <c r="K19" s="152"/>
-      <c r="L19" s="151"/>
-      <c r="M19" s="152"/>
-      <c r="N19" s="153"/>
-      <c r="O19" s="154"/>
-      <c r="P19" s="151"/>
-      <c r="Q19" s="152"/>
-      <c r="R19" s="151"/>
-      <c r="S19" s="152"/>
-      <c r="T19" s="151"/>
-      <c r="U19" s="152"/>
-      <c r="V19" s="155"/>
-      <c r="W19" s="156"/>
-      <c r="X19" s="157"/>
-      <c r="Y19" s="158"/>
-      <c r="Z19" s="157"/>
-      <c r="AA19" s="158"/>
-      <c r="AB19" s="157"/>
-      <c r="AC19" s="158"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="107"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="141"/>
+      <c r="O19" s="142"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="108"/>
+      <c r="R19" s="107"/>
+      <c r="S19" s="108"/>
+      <c r="T19" s="107"/>
+      <c r="U19" s="108"/>
+      <c r="V19" s="125"/>
+      <c r="W19" s="126"/>
+      <c r="X19" s="127"/>
+      <c r="Y19" s="128"/>
+      <c r="Z19" s="127"/>
+      <c r="AA19" s="128"/>
+      <c r="AB19" s="127"/>
+      <c r="AC19" s="128"/>
       <c r="AD19" s="54"/>
       <c r="AE19" s="63"/>
-      <c r="AG19" s="149"/>
-      <c r="AH19" s="150"/>
+      <c r="AG19" s="140"/>
+      <c r="AH19" s="137"/>
     </row>
     <row r="20" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="55"/>
@@ -5794,33 +5794,33 @@
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
       <c r="E20" s="53"/>
-      <c r="F20" s="151">
+      <c r="F20" s="107">
         <f>F19</f>
         <v>0</v>
       </c>
-      <c r="G20" s="152"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="152"/>
-      <c r="J20" s="151"/>
-      <c r="K20" s="152"/>
-      <c r="L20" s="151"/>
-      <c r="M20" s="152"/>
-      <c r="N20" s="151"/>
-      <c r="O20" s="152"/>
-      <c r="P20" s="151"/>
-      <c r="Q20" s="152"/>
-      <c r="R20" s="151"/>
-      <c r="S20" s="152"/>
-      <c r="T20" s="151"/>
-      <c r="U20" s="152"/>
-      <c r="V20" s="151"/>
-      <c r="W20" s="152"/>
-      <c r="X20" s="151"/>
-      <c r="Y20" s="152"/>
-      <c r="Z20" s="151"/>
-      <c r="AA20" s="152"/>
-      <c r="AB20" s="151"/>
-      <c r="AC20" s="152"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="107"/>
+      <c r="O20" s="108"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="108"/>
+      <c r="R20" s="107"/>
+      <c r="S20" s="108"/>
+      <c r="T20" s="107"/>
+      <c r="U20" s="108"/>
+      <c r="V20" s="107"/>
+      <c r="W20" s="108"/>
+      <c r="X20" s="107"/>
+      <c r="Y20" s="108"/>
+      <c r="Z20" s="107"/>
+      <c r="AA20" s="108"/>
+      <c r="AB20" s="107"/>
+      <c r="AC20" s="108"/>
       <c r="AD20" s="53"/>
       <c r="AE20" s="63"/>
     </row>
@@ -5832,30 +5832,30 @@
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
       <c r="E21" s="53"/>
-      <c r="F21" s="159"/>
-      <c r="G21" s="159"/>
-      <c r="H21" s="159"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
-      <c r="K21" s="159"/>
-      <c r="L21" s="159"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="159"/>
-      <c r="O21" s="159"/>
-      <c r="P21" s="159"/>
-      <c r="Q21" s="159"/>
-      <c r="R21" s="159"/>
-      <c r="S21" s="159"/>
-      <c r="T21" s="159"/>
-      <c r="U21" s="159"/>
-      <c r="V21" s="159"/>
-      <c r="W21" s="159"/>
-      <c r="X21" s="159"/>
-      <c r="Y21" s="159"/>
-      <c r="Z21" s="159"/>
-      <c r="AA21" s="159"/>
-      <c r="AB21" s="159"/>
-      <c r="AC21" s="159"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
+      <c r="T21" s="111"/>
+      <c r="U21" s="111"/>
+      <c r="V21" s="111"/>
+      <c r="W21" s="111"/>
+      <c r="X21" s="111"/>
+      <c r="Y21" s="111"/>
+      <c r="Z21" s="111"/>
+      <c r="AA21" s="111"/>
+      <c r="AB21" s="111"/>
+      <c r="AC21" s="111"/>
       <c r="AD21" s="53"/>
       <c r="AE21" s="63"/>
     </row>
@@ -5869,30 +5869,30 @@
         <v>0.03</v>
       </c>
       <c r="E22" s="53"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="163"/>
-      <c r="H22" s="162"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="162"/>
-      <c r="K22" s="163"/>
-      <c r="L22" s="162"/>
-      <c r="M22" s="163"/>
-      <c r="N22" s="162"/>
-      <c r="O22" s="163"/>
-      <c r="P22" s="162"/>
-      <c r="Q22" s="163"/>
-      <c r="R22" s="162"/>
-      <c r="S22" s="163"/>
-      <c r="T22" s="162"/>
-      <c r="U22" s="163"/>
-      <c r="V22" s="162"/>
-      <c r="W22" s="163"/>
-      <c r="X22" s="162"/>
-      <c r="Y22" s="163"/>
-      <c r="Z22" s="162"/>
-      <c r="AA22" s="163"/>
-      <c r="AB22" s="162"/>
-      <c r="AC22" s="163"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="122"/>
+      <c r="I22" s="123"/>
+      <c r="J22" s="122"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="122"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="122"/>
+      <c r="O22" s="123"/>
+      <c r="P22" s="122"/>
+      <c r="Q22" s="123"/>
+      <c r="R22" s="122"/>
+      <c r="S22" s="123"/>
+      <c r="T22" s="122"/>
+      <c r="U22" s="123"/>
+      <c r="V22" s="122"/>
+      <c r="W22" s="123"/>
+      <c r="X22" s="122"/>
+      <c r="Y22" s="123"/>
+      <c r="Z22" s="122"/>
+      <c r="AA22" s="123"/>
+      <c r="AB22" s="122"/>
+      <c r="AC22" s="123"/>
       <c r="AD22" s="53"/>
       <c r="AE22" s="63"/>
     </row>
@@ -5904,34 +5904,34 @@
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="53"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="160"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="160"/>
-      <c r="K23" s="161"/>
-      <c r="L23" s="160"/>
-      <c r="M23" s="164"/>
-      <c r="N23" s="160"/>
-      <c r="O23" s="161"/>
-      <c r="P23" s="160"/>
-      <c r="Q23" s="161"/>
-      <c r="R23" s="160"/>
-      <c r="S23" s="161"/>
-      <c r="T23" s="160"/>
-      <c r="U23" s="161"/>
-      <c r="V23" s="160"/>
-      <c r="W23" s="161"/>
-      <c r="X23" s="160"/>
-      <c r="Y23" s="161"/>
-      <c r="Z23" s="160"/>
-      <c r="AA23" s="164"/>
-      <c r="AB23" s="160"/>
-      <c r="AC23" s="161"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="124"/>
+      <c r="N23" s="112"/>
+      <c r="O23" s="113"/>
+      <c r="P23" s="112"/>
+      <c r="Q23" s="113"/>
+      <c r="R23" s="112"/>
+      <c r="S23" s="113"/>
+      <c r="T23" s="112"/>
+      <c r="U23" s="113"/>
+      <c r="V23" s="112"/>
+      <c r="W23" s="113"/>
+      <c r="X23" s="112"/>
+      <c r="Y23" s="113"/>
+      <c r="Z23" s="112"/>
+      <c r="AA23" s="124"/>
+      <c r="AB23" s="112"/>
+      <c r="AC23" s="113"/>
       <c r="AD23" s="53"/>
       <c r="AE23" s="63"/>
-      <c r="AG23" s="149"/>
-      <c r="AH23" s="150"/>
+      <c r="AG23" s="140"/>
+      <c r="AH23" s="137"/>
     </row>
     <row r="24" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="55"/>
@@ -5941,33 +5941,33 @@
       <c r="C24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="53"/>
-      <c r="F24" s="151">
+      <c r="F24" s="107">
         <f>F23</f>
         <v>0</v>
       </c>
-      <c r="G24" s="152"/>
-      <c r="H24" s="151"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="151"/>
-      <c r="K24" s="152"/>
-      <c r="L24" s="151"/>
-      <c r="M24" s="152"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="152"/>
-      <c r="P24" s="151"/>
-      <c r="Q24" s="152"/>
-      <c r="R24" s="151"/>
-      <c r="S24" s="152"/>
-      <c r="T24" s="151"/>
-      <c r="U24" s="152"/>
-      <c r="V24" s="151"/>
-      <c r="W24" s="152"/>
-      <c r="X24" s="151"/>
-      <c r="Y24" s="152"/>
-      <c r="Z24" s="151"/>
-      <c r="AA24" s="152"/>
-      <c r="AB24" s="151"/>
-      <c r="AC24" s="152"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="108"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="108"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="107"/>
+      <c r="O24" s="108"/>
+      <c r="P24" s="107"/>
+      <c r="Q24" s="108"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="107"/>
+      <c r="U24" s="108"/>
+      <c r="V24" s="107"/>
+      <c r="W24" s="108"/>
+      <c r="X24" s="107"/>
+      <c r="Y24" s="108"/>
+      <c r="Z24" s="107"/>
+      <c r="AA24" s="108"/>
+      <c r="AB24" s="107"/>
+      <c r="AC24" s="108"/>
       <c r="AD24" s="53"/>
       <c r="AE24" s="63"/>
     </row>
@@ -5977,30 +5977,30 @@
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="81"/>
-      <c r="F25" s="151"/>
-      <c r="G25" s="152"/>
-      <c r="H25" s="151"/>
-      <c r="I25" s="152"/>
-      <c r="J25" s="151"/>
-      <c r="K25" s="152"/>
-      <c r="L25" s="151"/>
-      <c r="M25" s="152"/>
-      <c r="N25" s="151"/>
-      <c r="O25" s="152"/>
-      <c r="P25" s="151"/>
-      <c r="Q25" s="152"/>
-      <c r="R25" s="151"/>
-      <c r="S25" s="152"/>
-      <c r="T25" s="151"/>
-      <c r="U25" s="152"/>
-      <c r="V25" s="151"/>
-      <c r="W25" s="152"/>
-      <c r="X25" s="151"/>
-      <c r="Y25" s="152"/>
-      <c r="Z25" s="151"/>
-      <c r="AA25" s="152"/>
-      <c r="AB25" s="151"/>
-      <c r="AC25" s="152"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="108"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="108"/>
+      <c r="N25" s="107"/>
+      <c r="O25" s="108"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="107"/>
+      <c r="S25" s="108"/>
+      <c r="T25" s="107"/>
+      <c r="U25" s="108"/>
+      <c r="V25" s="107"/>
+      <c r="W25" s="108"/>
+      <c r="X25" s="107"/>
+      <c r="Y25" s="108"/>
+      <c r="Z25" s="107"/>
+      <c r="AA25" s="108"/>
+      <c r="AB25" s="107"/>
+      <c r="AC25" s="108"/>
       <c r="AD25" s="82"/>
       <c r="AE25" s="63"/>
     </row>
@@ -6027,16 +6027,16 @@
       <c r="R26" s="47"/>
       <c r="S26" s="47"/>
       <c r="T26" s="65"/>
-      <c r="U26" s="168"/>
-      <c r="V26" s="169"/>
-      <c r="W26" s="169"/>
-      <c r="X26" s="170"/>
+      <c r="U26" s="119"/>
+      <c r="V26" s="120"/>
+      <c r="W26" s="120"/>
+      <c r="X26" s="121"/>
       <c r="Y26" s="65"/>
       <c r="Z26" s="44"/>
       <c r="AA26" s="65"/>
       <c r="AB26" s="73"/>
-      <c r="AC26" s="171"/>
-      <c r="AD26" s="172"/>
+      <c r="AC26" s="115"/>
+      <c r="AD26" s="116"/>
       <c r="AE26" s="63"/>
     </row>
     <row r="27" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6063,13 +6063,13 @@
       <c r="U27" s="28"/>
       <c r="V27" s="28"/>
       <c r="W27" s="28"/>
-      <c r="X27" s="165"/>
-      <c r="Y27" s="166"/>
-      <c r="Z27" s="166"/>
-      <c r="AA27" s="166"/>
-      <c r="AB27" s="166"/>
-      <c r="AC27" s="166"/>
-      <c r="AD27" s="166"/>
+      <c r="X27" s="114"/>
+      <c r="Y27" s="129"/>
+      <c r="Z27" s="129"/>
+      <c r="AA27" s="129"/>
+      <c r="AB27" s="129"/>
+      <c r="AC27" s="129"/>
+      <c r="AD27" s="129"/>
       <c r="AE27" s="56"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -6173,9 +6173,9 @@
     </row>
     <row r="31" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
-      <c r="B31" s="167"/>
-      <c r="C31" s="167"/>
-      <c r="D31" s="167"/>
+      <c r="B31" s="143"/>
+      <c r="C31" s="143"/>
+      <c r="D31" s="143"/>
       <c r="E31" s="22"/>
       <c r="F31" s="23"/>
       <c r="G31" s="24"/>
@@ -6277,32 +6277,32 @@
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="51"/>
-      <c r="E34" s="142"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="148"/>
-      <c r="I34" s="142"/>
-      <c r="J34" s="148"/>
-      <c r="K34" s="142"/>
-      <c r="L34" s="148"/>
-      <c r="M34" s="142"/>
-      <c r="N34" s="148"/>
-      <c r="O34" s="142"/>
-      <c r="P34" s="148"/>
-      <c r="Q34" s="142"/>
-      <c r="R34" s="148"/>
-      <c r="S34" s="142"/>
-      <c r="T34" s="148"/>
-      <c r="U34" s="142"/>
-      <c r="V34" s="148"/>
-      <c r="W34" s="142"/>
-      <c r="X34" s="148"/>
-      <c r="Y34" s="142"/>
-      <c r="Z34" s="148"/>
-      <c r="AA34" s="142"/>
-      <c r="AB34" s="148"/>
-      <c r="AC34" s="142"/>
-      <c r="AD34" s="148"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="118"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="118"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="118"/>
+      <c r="O34" s="117"/>
+      <c r="P34" s="118"/>
+      <c r="Q34" s="117"/>
+      <c r="R34" s="118"/>
+      <c r="S34" s="117"/>
+      <c r="T34" s="118"/>
+      <c r="U34" s="117"/>
+      <c r="V34" s="118"/>
+      <c r="W34" s="117"/>
+      <c r="X34" s="118"/>
+      <c r="Y34" s="117"/>
+      <c r="Z34" s="118"/>
+      <c r="AA34" s="117"/>
+      <c r="AB34" s="118"/>
+      <c r="AC34" s="117"/>
+      <c r="AD34" s="118"/>
       <c r="AE34" s="56"/>
     </row>
     <row r="35" spans="1:35" ht="15.6" x14ac:dyDescent="0.25">
@@ -6314,30 +6314,30 @@
       <c r="D35" s="24"/>
       <c r="E35" s="144"/>
       <c r="F35" s="145"/>
-      <c r="G35" s="146"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="146"/>
-      <c r="J35" s="147"/>
-      <c r="K35" s="146"/>
-      <c r="L35" s="147"/>
-      <c r="M35" s="146"/>
-      <c r="N35" s="147"/>
-      <c r="O35" s="146"/>
-      <c r="P35" s="147"/>
-      <c r="Q35" s="146"/>
-      <c r="R35" s="147"/>
-      <c r="S35" s="146"/>
-      <c r="T35" s="147"/>
-      <c r="U35" s="146"/>
-      <c r="V35" s="147"/>
-      <c r="W35" s="146"/>
-      <c r="X35" s="147"/>
-      <c r="Y35" s="146"/>
-      <c r="Z35" s="147"/>
-      <c r="AA35" s="146"/>
-      <c r="AB35" s="147"/>
-      <c r="AC35" s="146"/>
-      <c r="AD35" s="147"/>
+      <c r="G35" s="109"/>
+      <c r="H35" s="110"/>
+      <c r="I35" s="109"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="109"/>
+      <c r="L35" s="110"/>
+      <c r="M35" s="109"/>
+      <c r="N35" s="110"/>
+      <c r="O35" s="109"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="109"/>
+      <c r="R35" s="110"/>
+      <c r="S35" s="109"/>
+      <c r="T35" s="110"/>
+      <c r="U35" s="109"/>
+      <c r="V35" s="110"/>
+      <c r="W35" s="109"/>
+      <c r="X35" s="110"/>
+      <c r="Y35" s="109"/>
+      <c r="Z35" s="110"/>
+      <c r="AA35" s="109"/>
+      <c r="AB35" s="110"/>
+      <c r="AC35" s="109"/>
+      <c r="AD35" s="110"/>
       <c r="AE35" s="56"/>
     </row>
     <row r="36" spans="1:35" ht="15.6" x14ac:dyDescent="0.25">
@@ -6347,32 +6347,32 @@
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="100"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="100"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="100"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="100"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="100"/>
-      <c r="Q36" s="99"/>
-      <c r="R36" s="100"/>
-      <c r="S36" s="99"/>
-      <c r="T36" s="100"/>
-      <c r="U36" s="99"/>
-      <c r="V36" s="100"/>
-      <c r="W36" s="99"/>
-      <c r="X36" s="100"/>
-      <c r="Y36" s="99"/>
-      <c r="Z36" s="100"/>
-      <c r="AA36" s="99"/>
-      <c r="AB36" s="100"/>
-      <c r="AC36" s="99"/>
-      <c r="AD36" s="100"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="181"/>
+      <c r="G36" s="106"/>
+      <c r="H36" s="181"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="181"/>
+      <c r="K36" s="106"/>
+      <c r="L36" s="181"/>
+      <c r="M36" s="106"/>
+      <c r="N36" s="181"/>
+      <c r="O36" s="106"/>
+      <c r="P36" s="181"/>
+      <c r="Q36" s="106"/>
+      <c r="R36" s="181"/>
+      <c r="S36" s="106"/>
+      <c r="T36" s="181"/>
+      <c r="U36" s="106"/>
+      <c r="V36" s="181"/>
+      <c r="W36" s="106"/>
+      <c r="X36" s="181"/>
+      <c r="Y36" s="106"/>
+      <c r="Z36" s="181"/>
+      <c r="AA36" s="106"/>
+      <c r="AB36" s="181"/>
+      <c r="AC36" s="106"/>
+      <c r="AD36" s="181"/>
       <c r="AE36" s="56"/>
     </row>
     <row r="37" spans="1:35" ht="15" x14ac:dyDescent="0.25">
@@ -6383,34 +6383,34 @@
       <c r="C37" s="52"/>
       <c r="D37" s="52"/>
       <c r="E37" s="54"/>
-      <c r="F37" s="151"/>
-      <c r="G37" s="152"/>
-      <c r="H37" s="151"/>
-      <c r="I37" s="152"/>
-      <c r="J37" s="151"/>
-      <c r="K37" s="152"/>
-      <c r="L37" s="151"/>
-      <c r="M37" s="152"/>
-      <c r="N37" s="153"/>
-      <c r="O37" s="154"/>
-      <c r="P37" s="151"/>
-      <c r="Q37" s="152"/>
-      <c r="R37" s="151"/>
-      <c r="S37" s="152"/>
-      <c r="T37" s="151"/>
-      <c r="U37" s="152"/>
-      <c r="V37" s="155"/>
-      <c r="W37" s="156"/>
-      <c r="X37" s="157"/>
-      <c r="Y37" s="158"/>
-      <c r="Z37" s="157"/>
-      <c r="AA37" s="158"/>
-      <c r="AB37" s="157"/>
-      <c r="AC37" s="158"/>
+      <c r="F37" s="107"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="107"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="107"/>
+      <c r="K37" s="108"/>
+      <c r="L37" s="107"/>
+      <c r="M37" s="108"/>
+      <c r="N37" s="141"/>
+      <c r="O37" s="142"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="108"/>
+      <c r="R37" s="107"/>
+      <c r="S37" s="108"/>
+      <c r="T37" s="107"/>
+      <c r="U37" s="108"/>
+      <c r="V37" s="125"/>
+      <c r="W37" s="126"/>
+      <c r="X37" s="127"/>
+      <c r="Y37" s="128"/>
+      <c r="Z37" s="127"/>
+      <c r="AA37" s="128"/>
+      <c r="AB37" s="127"/>
+      <c r="AC37" s="128"/>
       <c r="AD37" s="54"/>
       <c r="AE37" s="56"/>
-      <c r="AG37" s="149"/>
-      <c r="AH37" s="150"/>
+      <c r="AG37" s="140"/>
+      <c r="AH37" s="137"/>
     </row>
     <row r="38" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="55"/>
@@ -6420,37 +6420,37 @@
       <c r="C38" s="45"/>
       <c r="D38" s="45"/>
       <c r="E38" s="53"/>
-      <c r="F38" s="151">
+      <c r="F38" s="107">
         <f>F37+AB20</f>
         <v>0</v>
       </c>
-      <c r="G38" s="152"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="152"/>
-      <c r="J38" s="151"/>
-      <c r="K38" s="152"/>
-      <c r="L38" s="151"/>
-      <c r="M38" s="152"/>
-      <c r="N38" s="151"/>
-      <c r="O38" s="152"/>
-      <c r="P38" s="151"/>
-      <c r="Q38" s="152"/>
-      <c r="R38" s="151"/>
-      <c r="S38" s="152"/>
-      <c r="T38" s="151"/>
-      <c r="U38" s="152"/>
-      <c r="V38" s="151"/>
-      <c r="W38" s="152"/>
-      <c r="X38" s="151"/>
-      <c r="Y38" s="152"/>
-      <c r="Z38" s="151"/>
-      <c r="AA38" s="152"/>
-      <c r="AB38" s="151"/>
-      <c r="AC38" s="152"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="108"/>
+      <c r="J38" s="107"/>
+      <c r="K38" s="108"/>
+      <c r="L38" s="107"/>
+      <c r="M38" s="108"/>
+      <c r="N38" s="107"/>
+      <c r="O38" s="108"/>
+      <c r="P38" s="107"/>
+      <c r="Q38" s="108"/>
+      <c r="R38" s="107"/>
+      <c r="S38" s="108"/>
+      <c r="T38" s="107"/>
+      <c r="U38" s="108"/>
+      <c r="V38" s="107"/>
+      <c r="W38" s="108"/>
+      <c r="X38" s="107"/>
+      <c r="Y38" s="108"/>
+      <c r="Z38" s="107"/>
+      <c r="AA38" s="108"/>
+      <c r="AB38" s="107"/>
+      <c r="AC38" s="108"/>
       <c r="AD38" s="53"/>
       <c r="AE38" s="56"/>
-      <c r="AG38" s="149"/>
-      <c r="AH38" s="149"/>
+      <c r="AG38" s="140"/>
+      <c r="AH38" s="140"/>
     </row>
     <row r="39" spans="1:35" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="55"/>
@@ -6460,30 +6460,30 @@
       <c r="C39" s="45"/>
       <c r="D39" s="45"/>
       <c r="E39" s="53"/>
-      <c r="F39" s="159"/>
-      <c r="G39" s="159"/>
-      <c r="H39" s="159"/>
-      <c r="I39" s="159"/>
-      <c r="J39" s="159"/>
-      <c r="K39" s="159"/>
-      <c r="L39" s="159"/>
-      <c r="M39" s="159"/>
-      <c r="N39" s="159"/>
-      <c r="O39" s="159"/>
-      <c r="P39" s="159"/>
-      <c r="Q39" s="159"/>
-      <c r="R39" s="159"/>
-      <c r="S39" s="159"/>
-      <c r="T39" s="159"/>
-      <c r="U39" s="159"/>
-      <c r="V39" s="159"/>
-      <c r="W39" s="159"/>
-      <c r="X39" s="159"/>
-      <c r="Y39" s="159"/>
-      <c r="Z39" s="159"/>
-      <c r="AA39" s="159"/>
-      <c r="AB39" s="159"/>
-      <c r="AC39" s="159"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111"/>
+      <c r="H39" s="111"/>
+      <c r="I39" s="111"/>
+      <c r="J39" s="111"/>
+      <c r="K39" s="111"/>
+      <c r="L39" s="111"/>
+      <c r="M39" s="111"/>
+      <c r="N39" s="111"/>
+      <c r="O39" s="111"/>
+      <c r="P39" s="111"/>
+      <c r="Q39" s="111"/>
+      <c r="R39" s="111"/>
+      <c r="S39" s="111"/>
+      <c r="T39" s="111"/>
+      <c r="U39" s="111"/>
+      <c r="V39" s="111"/>
+      <c r="W39" s="111"/>
+      <c r="X39" s="111"/>
+      <c r="Y39" s="111"/>
+      <c r="Z39" s="111"/>
+      <c r="AA39" s="111"/>
+      <c r="AB39" s="111"/>
+      <c r="AC39" s="111"/>
       <c r="AD39" s="53"/>
       <c r="AE39" s="56"/>
     </row>
@@ -6497,30 +6497,30 @@
         <v>0.03</v>
       </c>
       <c r="E40" s="53"/>
-      <c r="F40" s="162"/>
-      <c r="G40" s="163"/>
-      <c r="H40" s="162"/>
-      <c r="I40" s="163"/>
-      <c r="J40" s="162"/>
-      <c r="K40" s="163"/>
-      <c r="L40" s="162"/>
-      <c r="M40" s="163"/>
-      <c r="N40" s="162"/>
-      <c r="O40" s="163"/>
-      <c r="P40" s="162"/>
-      <c r="Q40" s="163"/>
-      <c r="R40" s="162"/>
-      <c r="S40" s="163"/>
-      <c r="T40" s="162"/>
-      <c r="U40" s="163"/>
-      <c r="V40" s="162"/>
-      <c r="W40" s="163"/>
-      <c r="X40" s="162"/>
-      <c r="Y40" s="163"/>
-      <c r="Z40" s="162"/>
-      <c r="AA40" s="163"/>
-      <c r="AB40" s="162"/>
-      <c r="AC40" s="163"/>
+      <c r="F40" s="122"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="122"/>
+      <c r="I40" s="123"/>
+      <c r="J40" s="122"/>
+      <c r="K40" s="123"/>
+      <c r="L40" s="122"/>
+      <c r="M40" s="123"/>
+      <c r="N40" s="122"/>
+      <c r="O40" s="123"/>
+      <c r="P40" s="122"/>
+      <c r="Q40" s="123"/>
+      <c r="R40" s="122"/>
+      <c r="S40" s="123"/>
+      <c r="T40" s="122"/>
+      <c r="U40" s="123"/>
+      <c r="V40" s="122"/>
+      <c r="W40" s="123"/>
+      <c r="X40" s="122"/>
+      <c r="Y40" s="123"/>
+      <c r="Z40" s="122"/>
+      <c r="AA40" s="123"/>
+      <c r="AB40" s="122"/>
+      <c r="AC40" s="123"/>
       <c r="AD40" s="53"/>
       <c r="AE40" s="56"/>
     </row>
@@ -6532,30 +6532,30 @@
       <c r="C41" s="50"/>
       <c r="D41" s="50"/>
       <c r="E41" s="53"/>
-      <c r="F41" s="160"/>
-      <c r="G41" s="161"/>
-      <c r="H41" s="160"/>
-      <c r="I41" s="161"/>
-      <c r="J41" s="160"/>
-      <c r="K41" s="161"/>
-      <c r="L41" s="160"/>
-      <c r="M41" s="164"/>
-      <c r="N41" s="160"/>
-      <c r="O41" s="161"/>
-      <c r="P41" s="160"/>
-      <c r="Q41" s="161"/>
-      <c r="R41" s="160"/>
-      <c r="S41" s="161"/>
-      <c r="T41" s="160"/>
-      <c r="U41" s="161"/>
-      <c r="V41" s="160"/>
-      <c r="W41" s="161"/>
-      <c r="X41" s="160"/>
-      <c r="Y41" s="161"/>
-      <c r="Z41" s="160"/>
-      <c r="AA41" s="164"/>
-      <c r="AB41" s="160"/>
-      <c r="AC41" s="161"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="113"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="113"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="113"/>
+      <c r="L41" s="112"/>
+      <c r="M41" s="124"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="113"/>
+      <c r="P41" s="112"/>
+      <c r="Q41" s="113"/>
+      <c r="R41" s="112"/>
+      <c r="S41" s="113"/>
+      <c r="T41" s="112"/>
+      <c r="U41" s="113"/>
+      <c r="V41" s="112"/>
+      <c r="W41" s="113"/>
+      <c r="X41" s="112"/>
+      <c r="Y41" s="113"/>
+      <c r="Z41" s="112"/>
+      <c r="AA41" s="124"/>
+      <c r="AB41" s="112"/>
+      <c r="AC41" s="113"/>
       <c r="AD41" s="53"/>
       <c r="AE41" s="56"/>
     </row>
@@ -6567,33 +6567,33 @@
       <c r="C42" s="50"/>
       <c r="D42" s="50"/>
       <c r="E42" s="53"/>
-      <c r="F42" s="151">
+      <c r="F42" s="107">
         <f>F41+AB24</f>
         <v>0</v>
       </c>
-      <c r="G42" s="152"/>
-      <c r="H42" s="151"/>
-      <c r="I42" s="152"/>
-      <c r="J42" s="151"/>
-      <c r="K42" s="152"/>
-      <c r="L42" s="151"/>
-      <c r="M42" s="152"/>
-      <c r="N42" s="151"/>
-      <c r="O42" s="152"/>
-      <c r="P42" s="151"/>
-      <c r="Q42" s="152"/>
-      <c r="R42" s="151"/>
-      <c r="S42" s="152"/>
-      <c r="T42" s="151"/>
-      <c r="U42" s="152"/>
-      <c r="V42" s="151"/>
-      <c r="W42" s="152"/>
-      <c r="X42" s="151"/>
-      <c r="Y42" s="152"/>
-      <c r="Z42" s="151"/>
-      <c r="AA42" s="152"/>
-      <c r="AB42" s="151"/>
-      <c r="AC42" s="152"/>
+      <c r="G42" s="108"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="108"/>
+      <c r="J42" s="107"/>
+      <c r="K42" s="108"/>
+      <c r="L42" s="107"/>
+      <c r="M42" s="108"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="108"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="108"/>
+      <c r="R42" s="107"/>
+      <c r="S42" s="108"/>
+      <c r="T42" s="107"/>
+      <c r="U42" s="108"/>
+      <c r="V42" s="107"/>
+      <c r="W42" s="108"/>
+      <c r="X42" s="107"/>
+      <c r="Y42" s="108"/>
+      <c r="Z42" s="107"/>
+      <c r="AA42" s="108"/>
+      <c r="AB42" s="107"/>
+      <c r="AC42" s="108"/>
       <c r="AD42" s="53"/>
       <c r="AE42" s="56"/>
     </row>
@@ -6603,30 +6603,30 @@
       <c r="C43" s="50"/>
       <c r="D43" s="50"/>
       <c r="E43" s="81"/>
-      <c r="F43" s="151"/>
-      <c r="G43" s="152"/>
-      <c r="H43" s="151"/>
-      <c r="I43" s="152"/>
-      <c r="J43" s="151"/>
-      <c r="K43" s="152"/>
-      <c r="L43" s="151"/>
-      <c r="M43" s="152"/>
-      <c r="N43" s="151"/>
-      <c r="O43" s="152"/>
-      <c r="P43" s="151"/>
-      <c r="Q43" s="152"/>
-      <c r="R43" s="151"/>
-      <c r="S43" s="152"/>
-      <c r="T43" s="151"/>
-      <c r="U43" s="152"/>
-      <c r="V43" s="151"/>
-      <c r="W43" s="152"/>
-      <c r="X43" s="151"/>
-      <c r="Y43" s="152"/>
-      <c r="Z43" s="151"/>
-      <c r="AA43" s="152"/>
-      <c r="AB43" s="151"/>
-      <c r="AC43" s="152"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="108"/>
+      <c r="J43" s="107"/>
+      <c r="K43" s="108"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="108"/>
+      <c r="N43" s="107"/>
+      <c r="O43" s="108"/>
+      <c r="P43" s="107"/>
+      <c r="Q43" s="108"/>
+      <c r="R43" s="107"/>
+      <c r="S43" s="108"/>
+      <c r="T43" s="107"/>
+      <c r="U43" s="108"/>
+      <c r="V43" s="107"/>
+      <c r="W43" s="108"/>
+      <c r="X43" s="107"/>
+      <c r="Y43" s="108"/>
+      <c r="Z43" s="107"/>
+      <c r="AA43" s="108"/>
+      <c r="AB43" s="107"/>
+      <c r="AC43" s="108"/>
       <c r="AD43" s="82"/>
       <c r="AE43" s="56"/>
     </row>
@@ -6653,19 +6653,19 @@
       <c r="R44" s="47"/>
       <c r="S44" s="47"/>
       <c r="T44" s="65"/>
-      <c r="U44" s="168"/>
-      <c r="V44" s="169"/>
-      <c r="W44" s="169"/>
-      <c r="X44" s="170"/>
+      <c r="U44" s="119"/>
+      <c r="V44" s="120"/>
+      <c r="W44" s="120"/>
+      <c r="X44" s="121"/>
       <c r="Y44" s="65"/>
       <c r="Z44" s="44"/>
       <c r="AA44" s="65"/>
       <c r="AB44" s="73"/>
-      <c r="AC44" s="171"/>
-      <c r="AD44" s="172"/>
+      <c r="AC44" s="115"/>
+      <c r="AD44" s="116"/>
       <c r="AE44" s="56"/>
-      <c r="AG44" s="150"/>
-      <c r="AH44" s="150"/>
+      <c r="AG44" s="137"/>
+      <c r="AH44" s="137"/>
     </row>
     <row r="45" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="55"/>
@@ -6689,8 +6689,8 @@
       <c r="S45" s="28"/>
       <c r="T45" s="70"/>
       <c r="U45" s="71"/>
-      <c r="V45" s="165"/>
-      <c r="W45" s="165"/>
+      <c r="V45" s="114"/>
+      <c r="W45" s="114"/>
       <c r="X45" s="42"/>
       <c r="Y45" s="42"/>
       <c r="Z45" s="42"/>
@@ -6722,27 +6722,27 @@
       <c r="S46" s="28"/>
       <c r="T46" s="69"/>
       <c r="U46" s="28"/>
-      <c r="V46" s="165"/>
-      <c r="W46" s="165"/>
-      <c r="X46" s="166"/>
-      <c r="Y46" s="166"/>
-      <c r="Z46" s="166"/>
-      <c r="AA46" s="166"/>
-      <c r="AB46" s="166"/>
-      <c r="AC46" s="166"/>
-      <c r="AD46" s="166"/>
+      <c r="V46" s="114"/>
+      <c r="W46" s="114"/>
+      <c r="X46" s="129"/>
+      <c r="Y46" s="129"/>
+      <c r="Z46" s="129"/>
+      <c r="AA46" s="129"/>
+      <c r="AB46" s="129"/>
+      <c r="AC46" s="129"/>
+      <c r="AD46" s="129"/>
       <c r="AE46" s="56"/>
       <c r="AG46" s="78"/>
       <c r="AH46" s="78"/>
     </row>
     <row r="47" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="55"/>
-      <c r="B47" s="166"/>
-      <c r="C47" s="166"/>
-      <c r="D47" s="166"/>
-      <c r="E47" s="166"/>
-      <c r="F47" s="166"/>
-      <c r="G47" s="166"/>
+      <c r="B47" s="129"/>
+      <c r="C47" s="129"/>
+      <c r="D47" s="129"/>
+      <c r="E47" s="129"/>
+      <c r="F47" s="129"/>
+      <c r="G47" s="129"/>
       <c r="H47" s="41"/>
       <c r="I47" s="3"/>
       <c r="J47" s="41"/>
@@ -6759,34 +6759,34 @@
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
       <c r="W47" s="41"/>
-      <c r="X47" s="166"/>
-      <c r="Y47" s="166"/>
-      <c r="Z47" s="166"/>
-      <c r="AA47" s="166"/>
-      <c r="AB47" s="166"/>
-      <c r="AC47" s="166"/>
-      <c r="AD47" s="166"/>
+      <c r="X47" s="129"/>
+      <c r="Y47" s="129"/>
+      <c r="Z47" s="129"/>
+      <c r="AA47" s="129"/>
+      <c r="AB47" s="129"/>
+      <c r="AC47" s="129"/>
+      <c r="AD47" s="129"/>
       <c r="AE47" s="56"/>
-      <c r="AG47" s="174"/>
-      <c r="AH47" s="174"/>
+      <c r="AG47" s="131"/>
+      <c r="AH47" s="131"/>
       <c r="AI47" s="78"/>
     </row>
     <row r="48" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="55"/>
-      <c r="B48" s="166"/>
-      <c r="C48" s="166"/>
-      <c r="D48" s="166"/>
-      <c r="E48" s="166"/>
-      <c r="F48" s="166"/>
-      <c r="G48" s="166"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="129"/>
+      <c r="D48" s="129"/>
+      <c r="E48" s="129"/>
+      <c r="F48" s="129"/>
+      <c r="G48" s="129"/>
       <c r="H48" s="41"/>
       <c r="I48" s="3"/>
       <c r="J48" s="41"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="61"/>
-      <c r="N48" s="181"/>
-      <c r="O48" s="181"/>
+      <c r="N48" s="139"/>
+      <c r="O48" s="139"/>
       <c r="P48" s="61"/>
       <c r="Q48" s="61"/>
       <c r="R48" s="61"/>
@@ -6795,34 +6795,34 @@
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
       <c r="W48" s="41"/>
-      <c r="X48" s="166"/>
-      <c r="Y48" s="166"/>
-      <c r="Z48" s="166"/>
-      <c r="AA48" s="166"/>
-      <c r="AB48" s="166"/>
-      <c r="AC48" s="166"/>
-      <c r="AD48" s="166"/>
+      <c r="X48" s="129"/>
+      <c r="Y48" s="129"/>
+      <c r="Z48" s="129"/>
+      <c r="AA48" s="129"/>
+      <c r="AB48" s="129"/>
+      <c r="AC48" s="129"/>
+      <c r="AD48" s="129"/>
       <c r="AE48" s="56"/>
-      <c r="AG48" s="174"/>
-      <c r="AH48" s="174"/>
+      <c r="AG48" s="131"/>
+      <c r="AH48" s="131"/>
       <c r="AI48" s="78"/>
     </row>
     <row r="49" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="55"/>
-      <c r="B49" s="166"/>
-      <c r="C49" s="166"/>
-      <c r="D49" s="166"/>
-      <c r="E49" s="166"/>
-      <c r="F49" s="166"/>
-      <c r="G49" s="166"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="129"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="129"/>
+      <c r="F49" s="129"/>
+      <c r="G49" s="129"/>
       <c r="H49" s="41"/>
       <c r="I49" s="3"/>
       <c r="J49" s="41"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="61"/>
-      <c r="N49" s="173"/>
-      <c r="O49" s="173"/>
+      <c r="N49" s="130"/>
+      <c r="O49" s="130"/>
       <c r="P49" s="61"/>
       <c r="Q49" s="61"/>
       <c r="R49" s="61"/>
@@ -6839,8 +6839,8 @@
       <c r="AC49" s="61"/>
       <c r="AD49" s="61"/>
       <c r="AE49" s="56"/>
-      <c r="AG49" s="174"/>
-      <c r="AH49" s="174"/>
+      <c r="AG49" s="131"/>
+      <c r="AH49" s="131"/>
       <c r="AI49" s="78"/>
     </row>
     <row r="50" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6875,8 +6875,8 @@
       <c r="AC50" s="61"/>
       <c r="AD50" s="61"/>
       <c r="AE50" s="56"/>
-      <c r="AG50" s="174"/>
-      <c r="AH50" s="174"/>
+      <c r="AG50" s="131"/>
+      <c r="AH50" s="131"/>
       <c r="AI50" s="78"/>
     </row>
     <row r="51" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6911,8 +6911,8 @@
       <c r="AC51" s="61"/>
       <c r="AD51" s="61"/>
       <c r="AE51" s="56"/>
-      <c r="AG51" s="174"/>
-      <c r="AH51" s="174"/>
+      <c r="AG51" s="131"/>
+      <c r="AH51" s="131"/>
       <c r="AI51" s="78"/>
     </row>
     <row r="52" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6947,8 +6947,8 @@
       <c r="AC52" s="61"/>
       <c r="AD52" s="61"/>
       <c r="AE52" s="56"/>
-      <c r="AG52" s="174"/>
-      <c r="AH52" s="174"/>
+      <c r="AG52" s="131"/>
+      <c r="AH52" s="131"/>
       <c r="AI52" s="78"/>
     </row>
     <row r="53" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6983,18 +6983,18 @@
       <c r="AC53" s="61"/>
       <c r="AD53" s="61"/>
       <c r="AE53" s="56"/>
-      <c r="AG53" s="174"/>
-      <c r="AH53" s="174"/>
+      <c r="AG53" s="131"/>
+      <c r="AH53" s="131"/>
       <c r="AI53" s="78"/>
     </row>
     <row r="54" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="55"/>
-      <c r="B54" s="173"/>
-      <c r="C54" s="173"/>
-      <c r="D54" s="173"/>
-      <c r="E54" s="173"/>
-      <c r="F54" s="173"/>
-      <c r="G54" s="173"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="130"/>
+      <c r="D54" s="130"/>
+      <c r="E54" s="130"/>
+      <c r="F54" s="130"/>
+      <c r="G54" s="130"/>
       <c r="H54" s="41"/>
       <c r="I54" s="3"/>
       <c r="J54" s="41"/>
@@ -7011,54 +7011,309 @@
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
       <c r="W54" s="41"/>
-      <c r="X54" s="166"/>
-      <c r="Y54" s="166"/>
-      <c r="Z54" s="166"/>
-      <c r="AA54" s="166"/>
-      <c r="AB54" s="166"/>
-      <c r="AC54" s="166"/>
-      <c r="AD54" s="166"/>
-      <c r="AE54" s="180"/>
-      <c r="AG54" s="150"/>
-      <c r="AH54" s="150"/>
+      <c r="X54" s="129"/>
+      <c r="Y54" s="129"/>
+      <c r="Z54" s="129"/>
+      <c r="AA54" s="129"/>
+      <c r="AB54" s="129"/>
+      <c r="AC54" s="129"/>
+      <c r="AD54" s="129"/>
+      <c r="AE54" s="138"/>
+      <c r="AG54" s="137"/>
+      <c r="AH54" s="137"/>
     </row>
     <row r="55" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="58"/>
-      <c r="B55" s="175"/>
-      <c r="C55" s="176"/>
-      <c r="D55" s="176"/>
-      <c r="E55" s="176"/>
-      <c r="F55" s="176"/>
-      <c r="G55" s="176"/>
+      <c r="B55" s="132"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="133"/>
+      <c r="E55" s="133"/>
+      <c r="F55" s="133"/>
+      <c r="G55" s="133"/>
       <c r="H55" s="64"/>
       <c r="I55" s="59"/>
-      <c r="J55" s="177"/>
-      <c r="K55" s="178"/>
+      <c r="J55" s="134"/>
+      <c r="K55" s="135"/>
       <c r="L55" s="74"/>
-      <c r="M55" s="176"/>
-      <c r="N55" s="176"/>
-      <c r="O55" s="176"/>
-      <c r="P55" s="176"/>
-      <c r="Q55" s="176"/>
-      <c r="R55" s="176"/>
+      <c r="M55" s="133"/>
+      <c r="N55" s="133"/>
+      <c r="O55" s="133"/>
+      <c r="P55" s="133"/>
+      <c r="Q55" s="133"/>
+      <c r="R55" s="133"/>
       <c r="S55" s="75"/>
       <c r="T55" s="59"/>
       <c r="U55" s="59"/>
       <c r="V55" s="59"/>
       <c r="W55" s="59"/>
-      <c r="X55" s="179"/>
-      <c r="Y55" s="179"/>
-      <c r="Z55" s="179"/>
-      <c r="AA55" s="179"/>
-      <c r="AB55" s="179"/>
-      <c r="AC55" s="179"/>
-      <c r="AD55" s="179"/>
+      <c r="X55" s="136"/>
+      <c r="Y55" s="136"/>
+      <c r="Z55" s="136"/>
+      <c r="AA55" s="136"/>
+      <c r="AB55" s="136"/>
+      <c r="AC55" s="136"/>
+      <c r="AD55" s="136"/>
       <c r="AE55" s="60"/>
-      <c r="AG55" s="150"/>
-      <c r="AH55" s="150"/>
+      <c r="AG55" s="137"/>
+      <c r="AH55" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="279">
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="E2:T2"/>
+    <mergeCell ref="E3:T3"/>
+    <mergeCell ref="E4:T4"/>
+    <mergeCell ref="E6:T8"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="A2:B6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="T20:U20"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="X20:Y20"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="AB19:AC19"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="AB21:AC21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="X24:Y24"/>
+    <mergeCell ref="Z24:AA24"/>
+    <mergeCell ref="AB24:AC24"/>
+    <mergeCell ref="AG23:AH23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="X23:Y23"/>
+    <mergeCell ref="Z23:AA23"/>
+    <mergeCell ref="AB23:AC23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="X27:AD27"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="W35:X35"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Z37:AA37"/>
+    <mergeCell ref="AB38:AC38"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AG37:AH37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="AB37:AC37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="AG44:AH44"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="AB40:AC40"/>
+    <mergeCell ref="AB41:AC41"/>
+    <mergeCell ref="AB42:AC42"/>
+    <mergeCell ref="AB43:AC43"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="AC44:AD44"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="AG38:AH38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="X38:Y38"/>
+    <mergeCell ref="Z38:AA38"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="AG49:AH49"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="M55:R55"/>
+    <mergeCell ref="X55:AD55"/>
+    <mergeCell ref="AG55:AH55"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="X46:AD46"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="X47:AD47"/>
+    <mergeCell ref="AG47:AH47"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="X54:AE54"/>
+    <mergeCell ref="AG54:AH54"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="AG52:AH52"/>
+    <mergeCell ref="AG53:AH53"/>
+    <mergeCell ref="X48:AD48"/>
+    <mergeCell ref="AG48:AH48"/>
+    <mergeCell ref="AG50:AH50"/>
+    <mergeCell ref="AG51:AH51"/>
+    <mergeCell ref="Z40:AA40"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="R42:S42"/>
+    <mergeCell ref="T42:U42"/>
+    <mergeCell ref="V42:W42"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="X39:Y39"/>
+    <mergeCell ref="Z39:AA39"/>
+    <mergeCell ref="V40:W40"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="V41:W41"/>
+    <mergeCell ref="V45:W45"/>
+    <mergeCell ref="AC26:AD26"/>
+    <mergeCell ref="AC34:AD34"/>
+    <mergeCell ref="AC35:AD35"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="X25:Y25"/>
+    <mergeCell ref="Z25:AA25"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="X43:Y43"/>
+    <mergeCell ref="Z43:AA43"/>
+    <mergeCell ref="V43:W43"/>
+    <mergeCell ref="W34:X34"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="AA34:AB34"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="X42:Y42"/>
+    <mergeCell ref="Z42:AA42"/>
+    <mergeCell ref="X40:Y40"/>
+    <mergeCell ref="Z41:AA41"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="V37:W37"/>
+    <mergeCell ref="X37:Y37"/>
+    <mergeCell ref="T39:U39"/>
+    <mergeCell ref="T40:U40"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="J25:K25"/>
@@ -7083,261 +7338,6 @@
     <mergeCell ref="Q35:R35"/>
     <mergeCell ref="R41:S41"/>
     <mergeCell ref="T41:U41"/>
-    <mergeCell ref="V45:W45"/>
-    <mergeCell ref="AC26:AD26"/>
-    <mergeCell ref="AC34:AD34"/>
-    <mergeCell ref="AC35:AD35"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="X25:Y25"/>
-    <mergeCell ref="Z25:AA25"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="X43:Y43"/>
-    <mergeCell ref="Z43:AA43"/>
-    <mergeCell ref="V43:W43"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="X42:Y42"/>
-    <mergeCell ref="Z42:AA42"/>
-    <mergeCell ref="X40:Y40"/>
-    <mergeCell ref="Z41:AA41"/>
-    <mergeCell ref="AA35:AB35"/>
-    <mergeCell ref="V37:W37"/>
-    <mergeCell ref="X37:Y37"/>
-    <mergeCell ref="T39:U39"/>
-    <mergeCell ref="T40:U40"/>
-    <mergeCell ref="Z40:AA40"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="R42:S42"/>
-    <mergeCell ref="T42:U42"/>
-    <mergeCell ref="V42:W42"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="Z39:AA39"/>
-    <mergeCell ref="V40:W40"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="V41:W41"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="AG49:AH49"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="M55:R55"/>
-    <mergeCell ref="X55:AD55"/>
-    <mergeCell ref="AG55:AH55"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="X46:AD46"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="X47:AD47"/>
-    <mergeCell ref="AG47:AH47"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="X54:AE54"/>
-    <mergeCell ref="AG54:AH54"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="AG52:AH52"/>
-    <mergeCell ref="AG53:AH53"/>
-    <mergeCell ref="X48:AD48"/>
-    <mergeCell ref="AG48:AH48"/>
-    <mergeCell ref="AG50:AH50"/>
-    <mergeCell ref="AG51:AH51"/>
-    <mergeCell ref="AG44:AH44"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="AB40:AC40"/>
-    <mergeCell ref="AB41:AC41"/>
-    <mergeCell ref="AB42:AC42"/>
-    <mergeCell ref="AB43:AC43"/>
-    <mergeCell ref="U44:X44"/>
-    <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="AG38:AH38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="V38:W38"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="Z38:AA38"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="Z37:AA37"/>
-    <mergeCell ref="AB38:AC38"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AG37:AH37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="AB37:AC37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="X27:AD27"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="W35:X35"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="X24:Y24"/>
-    <mergeCell ref="Z24:AA24"/>
-    <mergeCell ref="AB24:AC24"/>
-    <mergeCell ref="AG23:AH23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="X23:Y23"/>
-    <mergeCell ref="Z23:AA23"/>
-    <mergeCell ref="AB23:AC23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="X19:Y19"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="AB19:AC19"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="AB21:AC21"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="T20:U20"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="X20:Y20"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="A2:B6"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="E2:T2"/>
-    <mergeCell ref="E3:T3"/>
-    <mergeCell ref="E4:T4"/>
-    <mergeCell ref="E6:T8"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="Z8:AA8"/>
   </mergeCells>
   <pageMargins left="0.31496062992126" right="0" top="0.5" bottom="0" header="0.39370078740157499" footer="0.39370078740157499"/>
   <pageSetup paperSize="5" scale="67" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>